<commit_message>
conversion excel en json
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/uploadfile/situationEnim copie.xlsx
+++ b/src/main/java/com/example/uploadfile/situationEnim copie.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA90EAC0-F9DC-164D-A703-101E8A02E97E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3BC0E5-6D31-9B4A-8DBD-1D247779D3DE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="268">
   <si>
     <t>date</t>
   </si>
@@ -812,9 +812,6 @@
   </si>
   <si>
     <t>DIOUF ADAMA</t>
-  </si>
-  <si>
-    <t>caisse</t>
   </si>
   <si>
     <t>1275___MAME SEYNABOU NDIAYE</t>
@@ -839,7 +836,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0\ _C_F_A_-;\-* #,##0\ _C_F_A_-;_-* &quot;-&quot;\ _C_F_A_-;_-@_-"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -870,12 +867,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri (Corps)_x0000_"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -891,7 +882,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1156,21 +1147,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1240,10 +1222,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1566,13 +1544,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
@@ -1580,9 +1558,9 @@
     <col min="4" max="4" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1593,11 +1571,8 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="27" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16">
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1102020</v>
       </c>
@@ -1608,13 +1583,10 @@
         <v>54247</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E2" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="32">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>701913</v>
       </c>
@@ -1625,13 +1597,10 @@
         <v>108462</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E3" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>2111646</v>
       </c>
@@ -1642,13 +1611,10 @@
         <v>176596</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E4" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="32">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>2111334</v>
       </c>
@@ -1659,13 +1625,10 @@
         <v>21357</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E5" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="32">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>2111333</v>
       </c>
@@ -1676,13 +1639,10 @@
         <v>21357</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E6" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>2111332</v>
       </c>
@@ -1693,13 +1653,10 @@
         <v>21357</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E7" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>9600966</v>
       </c>
@@ -1710,13 +1667,10 @@
         <v>795000</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E8" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>9502886</v>
       </c>
@@ -1727,13 +1681,10 @@
         <v>122014</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E9" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>710233</v>
       </c>
@@ -1744,13 +1695,10 @@
         <v>43949</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E10" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>702495</v>
       </c>
@@ -1761,13 +1709,10 @@
         <v>67799</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E11" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>7225013</v>
       </c>
@@ -1778,13 +1723,10 @@
         <v>191716</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E12" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="32">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>1410757</v>
       </c>
@@ -1795,13 +1737,10 @@
         <v>312524</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E13" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>111832</v>
       </c>
@@ -1812,13 +1751,10 @@
         <v>323367</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E14" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>1510465</v>
       </c>
@@ -1829,13 +1765,10 @@
         <v>278459</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E15" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="32">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>1311322</v>
       </c>
@@ -1846,13 +1779,10 @@
         <v>396125</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E16" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>2010961</v>
       </c>
@@ -1863,13 +1793,10 @@
         <v>51774</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E17" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>601886</v>
       </c>
@@ -1880,13 +1807,10 @@
         <v>59908</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E18" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="48">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>9600137</v>
       </c>
@@ -1897,13 +1821,10 @@
         <v>804596</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E19" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>1300279</v>
       </c>
@@ -1914,13 +1835,10 @@
         <v>162690</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E20" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>1811852</v>
       </c>
@@ -1931,13 +1849,10 @@
         <v>59055</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E21" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>1811191</v>
       </c>
@@ -1948,13 +1863,10 @@
         <v>57842</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E22" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>1811190</v>
       </c>
@@ -1965,13 +1877,10 @@
         <v>57842</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E23" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>1811185</v>
       </c>
@@ -1982,13 +1891,10 @@
         <v>180329</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E24" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="32">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>10862</v>
       </c>
@@ -1999,13 +1905,10 @@
         <v>320093</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E25" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>501133</v>
       </c>
@@ -2016,13 +1919,10 @@
         <v>149131</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E26" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>811149</v>
       </c>
@@ -2033,13 +1933,10 @@
         <v>51269</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E27" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>1311362</v>
       </c>
@@ -2050,13 +1947,10 @@
         <v>14654</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E28" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>1801171</v>
       </c>
@@ -2067,13 +1961,10 @@
         <v>230286</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E29" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>701920</v>
       </c>
@@ -2084,13 +1975,10 @@
         <v>94916</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E30" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>510982</v>
       </c>
@@ -2101,13 +1989,10 @@
         <v>92981</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E31" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>1101205</v>
       </c>
@@ -2118,13 +2003,10 @@
         <v>13584</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E32" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>900378</v>
       </c>
@@ -2135,13 +2017,10 @@
         <v>52502</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E33" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="32">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>1410732</v>
       </c>
@@ -2152,13 +2031,10 @@
         <v>3127471</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E34" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>1510259</v>
       </c>
@@ -2169,13 +2045,10 @@
         <v>298808</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E35" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="32">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>1400227</v>
       </c>
@@ -2186,13 +2059,10 @@
         <v>40682</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E36" s="28">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>511288</v>
       </c>
@@ -2203,13 +2073,10 @@
         <v>21830</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E37" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>560011</v>
       </c>
@@ -2220,13 +2087,10 @@
         <v>305236</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E38" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>810128</v>
       </c>
@@ -2237,13 +2101,10 @@
         <v>96386</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E39" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>1201388</v>
       </c>
@@ -2254,13 +2115,10 @@
         <v>40682</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E40" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>1712147</v>
       </c>
@@ -2271,13 +2129,10 @@
         <v>43942</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E41" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="32">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>9900691</v>
       </c>
@@ -2288,13 +2143,10 @@
         <v>665534</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E42" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>1400250</v>
       </c>
@@ -2305,13 +2157,10 @@
         <v>40682</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E43" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>1410248</v>
       </c>
@@ -2322,13 +2171,10 @@
         <v>40288</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E44" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>1500453</v>
       </c>
@@ -2339,13 +2185,10 @@
         <v>40944</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E45" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>9511576</v>
       </c>
@@ -2356,13 +2199,10 @@
         <v>270346</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E46" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>1410773</v>
       </c>
@@ -2373,13 +2213,10 @@
         <v>36635</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E47" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="32">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>1400264</v>
       </c>
@@ -2390,13 +2227,10 @@
         <v>67799</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E48" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>501328</v>
       </c>
@@ -2407,13 +2241,10 @@
         <v>184107</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E49" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="32">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>2000447</v>
       </c>
@@ -2424,13 +2255,10 @@
         <v>468071</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E50" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>101404</v>
       </c>
@@ -2441,13 +2269,10 @@
         <v>81358</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E51" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>1315019</v>
       </c>
@@ -2458,13 +2283,10 @@
         <v>390655</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E52" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>1411856</v>
       </c>
@@ -2475,13 +2297,10 @@
         <v>85950</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E53" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>9802949</v>
       </c>
@@ -2492,13 +2311,10 @@
         <v>162690</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E54" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>111772</v>
       </c>
@@ -2509,13 +2325,10 @@
         <v>167990</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E55" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="32">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>1210449</v>
       </c>
@@ -2526,13 +2339,10 @@
         <v>119462</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E56" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>710515</v>
       </c>
@@ -2543,13 +2353,10 @@
         <v>195337</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E57" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="32">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>1400261</v>
       </c>
@@ -2560,13 +2367,10 @@
         <v>122014</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E58" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>311678</v>
       </c>
@@ -2577,13 +2381,10 @@
         <v>132057</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E59" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>1510270</v>
       </c>
@@ -2594,13 +2395,10 @@
         <v>67419</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E60" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>1510271</v>
       </c>
@@ -2611,13 +2409,10 @@
         <v>67419</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E61" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="32">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>1510269</v>
       </c>
@@ -2628,13 +2423,10 @@
         <v>67419</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E62" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="16">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>2000468</v>
       </c>
@@ -2645,13 +2437,10 @@
         <v>40938</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E63" s="28">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="32">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>9410411</v>
       </c>
@@ -2662,13 +2451,10 @@
         <v>81607</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="E64" s="28">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="16">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>9802458</v>
       </c>
@@ -2679,13 +2465,10 @@
         <v>54247</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="E65" s="28">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="16">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>2442</v>
       </c>
@@ -2696,13 +2479,10 @@
         <v>40682</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="E66" s="28">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="32">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>9802158</v>
       </c>
@@ -2713,13 +2493,10 @@
         <v>81358</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="E67" s="28">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="16">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>602329</v>
       </c>
@@ -2730,13 +2507,10 @@
         <v>81358</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="E68" s="28">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="16">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>1510266</v>
       </c>
@@ -2747,13 +2521,10 @@
         <v>210201</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="E69" s="28">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="16">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>510981</v>
       </c>
@@ -2764,13 +2535,10 @@
         <v>92981</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="E70" s="28">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="32">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>8360182</v>
       </c>
@@ -2781,13 +2549,10 @@
         <v>305538</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="E71" s="28">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="16">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>310127</v>
       </c>
@@ -2798,13 +2563,10 @@
         <v>214235</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E72" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="32">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>1300287</v>
       </c>
@@ -2815,13 +2577,10 @@
         <v>40682</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E73" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="32">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>1702289</v>
       </c>
@@ -2832,13 +2591,10 @@
         <v>36897</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E74" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>411896</v>
       </c>
@@ -2849,13 +2605,10 @@
         <v>553928</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E75" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="32">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>310015</v>
       </c>
@@ -2866,13 +2619,10 @@
         <v>444627</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E76" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>1001326</v>
       </c>
@@ -2883,13 +2633,10 @@
         <v>54247</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E77" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>1010872</v>
       </c>
@@ -2900,13 +2647,10 @@
         <v>174596</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E78" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>1701457</v>
       </c>
@@ -2917,13 +2661,10 @@
         <v>12981</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E79" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>2212187</v>
       </c>
@@ -2934,13 +2675,10 @@
         <v>30121</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E80" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>610533</v>
       </c>
@@ -2951,13 +2689,10 @@
         <v>47248</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E81" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="32">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>7960020</v>
       </c>
@@ -2968,13 +2703,10 @@
         <v>611083</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E82" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>610946</v>
       </c>
@@ -2985,13 +2717,10 @@
         <v>553928</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E83" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>9700876</v>
       </c>
@@ -3002,13 +2731,10 @@
         <v>149131</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E84" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="32">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>410260</v>
       </c>
@@ -3019,13 +2745,10 @@
         <v>137449</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E85" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="32">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>7411768</v>
       </c>
@@ -3036,13 +2759,10 @@
         <v>387992</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E86" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="32">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>2111331</v>
       </c>
@@ -3053,13 +2773,10 @@
         <v>21357</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E87" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>2212023</v>
       </c>
@@ -3070,13 +2787,10 @@
         <v>6188822</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E88" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>112295</v>
       </c>
@@ -3087,13 +2801,10 @@
         <v>218282</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E89" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>702472</v>
       </c>
@@ -3104,13 +2815,10 @@
         <v>81358</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E90" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>701937</v>
       </c>
@@ -3121,13 +2829,10 @@
         <v>94916</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E91" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>410905</v>
       </c>
@@ -3138,13 +2843,10 @@
         <v>132831</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E92" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="16">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>1111169</v>
       </c>
@@ -3155,21 +2857,18 @@
         <v>101574</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E93" s="28">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="6"/>
       <c r="D94" s="4"/>
     </row>
-    <row r="95" spans="1:5" ht="16" thickBot="1">
-      <c r="A95" s="29"/>
-      <c r="B95" s="30"/>
+    <row r="95" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="27"/>
+      <c r="B95" s="28"/>
       <c r="C95" s="7">
         <f>SUM(C2:C93)</f>
         <v>24114189</v>
@@ -3192,7 +2891,7 @@
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="9.1640625"/>
@@ -3201,7 +2900,7 @@
     <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34">
+    <row r="1" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3218,7 +2917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32">
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>44925</v>
       </c>
@@ -3235,7 +2934,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="32">
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4">
         <v>1611608</v>
@@ -3250,7 +2949,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32">
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="4">
         <v>211941</v>
@@ -3265,7 +2964,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="32">
+    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="4">
         <v>1102058</v>
@@ -3280,7 +2979,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="32">
+    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="4">
         <v>711692</v>
@@ -3295,7 +2994,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="32">
+    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="4">
         <v>1712046</v>
@@ -3310,7 +3009,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="32">
+    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="4">
         <v>9502702</v>
@@ -3325,7 +3024,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="32">
+    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="4">
         <v>1611061</v>
@@ -3340,7 +3039,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="32">
+    <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="4">
         <v>2111607</v>
@@ -3355,7 +3054,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="32">
+    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="4">
         <v>911399</v>
@@ -3370,7 +3069,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="32">
+    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="4">
         <v>611598</v>
@@ -3385,7 +3084,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="32">
+    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="4">
         <v>900403</v>
@@ -3400,7 +3099,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="32">
+    <row r="14" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="4">
         <v>1310907</v>
@@ -3415,7 +3114,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="32">
+    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="4">
         <v>1510395</v>
@@ -3430,7 +3129,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="32">
+    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="4">
         <v>201466</v>
@@ -3445,7 +3144,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="32">
+    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="4">
         <v>1711692</v>
@@ -3460,7 +3159,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="32">
+    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="4">
         <v>1001334</v>
@@ -3475,7 +3174,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="32">
+    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="4">
         <v>9912253</v>
@@ -3490,7 +3189,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="32">
+    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="4">
         <v>1010880</v>
@@ -3505,7 +3204,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="32">
+    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="4">
         <v>801241</v>
@@ -3520,7 +3219,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="32">
+    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="4">
         <v>1500370</v>
@@ -3535,7 +3234,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="32">
+    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="4">
         <v>1800733</v>
@@ -3550,7 +3249,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="32">
+    <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="4">
         <v>1212564</v>
@@ -3565,7 +3264,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="32">
+    <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="4">
         <v>11807</v>
@@ -3580,7 +3279,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="32">
+    <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="4">
         <v>300006</v>
@@ -3595,7 +3294,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="32">
+    <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="4">
         <v>1212563</v>
@@ -3610,7 +3309,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="32">
+    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="4">
         <v>1300269</v>
@@ -3625,7 +3324,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="32">
+    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="4">
         <v>1001356</v>
@@ -3640,7 +3339,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="32">
+    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="4">
         <v>9900905</v>
@@ -3655,7 +3354,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="32">
+    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="4">
         <v>2111603</v>
@@ -3670,12 +3369,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="16" thickBot="1">
-      <c r="A32" s="31" t="s">
+    <row r="32" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="30"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
       <c r="D32" s="7">
         <f>+SUM(D2:D30)</f>
         <v>3563051</v>
@@ -3700,15 +3399,15 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="36"/>
-    </row>
-    <row r="2" spans="1:11" ht="80">
+      <c r="B1" s="34"/>
+    </row>
+    <row r="2" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>98</v>
       </c>
@@ -3716,7 +3415,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="48">
+    <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>100</v>
       </c>
@@ -3724,8 +3423,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16" thickBot="1"/>
-    <row r="5" spans="1:11" ht="32">
+    <row r="4" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
@@ -3758,14 +3457,14 @@
       </c>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11" ht="16" thickBot="1">
-      <c r="A6" s="37" t="s">
+    <row r="6" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="39"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="14">
         <v>0</v>
       </c>
@@ -3775,17 +3474,17 @@
       <c r="H6" s="15">
         <v>0</v>
       </c>
-      <c r="I6" s="40"/>
-      <c r="J6" s="39"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="37"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="8" spans="1:11" ht="16" thickBot="1">
-      <c r="A8" s="41" t="s">
+    <row r="8" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="41"/>
-    </row>
-    <row r="9" spans="1:11" ht="32">
+      <c r="B8" s="39"/>
+    </row>
+    <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>0</v>
       </c>
@@ -3812,7 +3511,7 @@
       </c>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:11" ht="32">
+    <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>44925.663518518515</v>
       </c>
@@ -3839,7 +3538,7 @@
       </c>
       <c r="I10" s="17"/>
     </row>
-    <row r="11" spans="1:11" ht="32">
+    <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>44925.650625000002</v>
       </c>
@@ -3866,7 +3565,7 @@
       </c>
       <c r="I11" s="17"/>
     </row>
-    <row r="12" spans="1:11" ht="32">
+    <row r="12" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>44925.536261574074</v>
       </c>
@@ -3893,7 +3592,7 @@
       </c>
       <c r="I12" s="17"/>
     </row>
-    <row r="13" spans="1:11" ht="32">
+    <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>44925.525937500002</v>
       </c>
@@ -3920,7 +3619,7 @@
       </c>
       <c r="I13" s="17"/>
     </row>
-    <row r="14" spans="1:11" ht="48">
+    <row r="14" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>44925.52447916667</v>
       </c>
@@ -3947,7 +3646,7 @@
       </c>
       <c r="I14" s="17"/>
     </row>
-    <row r="15" spans="1:11" ht="32">
+    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>44925.52238425926</v>
       </c>
@@ -3974,7 +3673,7 @@
       </c>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:11" ht="32">
+    <row r="16" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>44925.51903935185</v>
       </c>
@@ -4001,7 +3700,7 @@
       </c>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="1:9" ht="32">
+    <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>44925.500601851854</v>
       </c>
@@ -4028,7 +3727,7 @@
       </c>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" ht="32">
+    <row r="18" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>44925.494479166664</v>
       </c>
@@ -4055,7 +3754,7 @@
       </c>
       <c r="I18" s="17"/>
     </row>
-    <row r="19" spans="1:9" ht="48">
+    <row r="19" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>44925.487453703703</v>
       </c>
@@ -4082,7 +3781,7 @@
       </c>
       <c r="I19" s="17"/>
     </row>
-    <row r="20" spans="1:9" ht="32">
+    <row r="20" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>44925.394594907404</v>
       </c>
@@ -4109,7 +3808,7 @@
       </c>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:9" ht="32">
+    <row r="21" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>44925.389467592591</v>
       </c>
@@ -4136,7 +3835,7 @@
       </c>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" ht="48">
+    <row r="22" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>44925.385300925926</v>
       </c>
@@ -4163,7 +3862,7 @@
       </c>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" ht="48">
+    <row r="23" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>44925.38177083333</v>
       </c>
@@ -4190,7 +3889,7 @@
       </c>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:9" ht="32">
+    <row r="24" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>44925.380150462966</v>
       </c>
@@ -4217,7 +3916,7 @@
       </c>
       <c r="I24" s="17"/>
     </row>
-    <row r="25" spans="1:9" ht="48">
+    <row r="25" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>44925.349317129629</v>
       </c>
@@ -4244,7 +3943,7 @@
       </c>
       <c r="I25" s="17"/>
     </row>
-    <row r="26" spans="1:9" ht="32">
+    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>44925.331030092595</v>
       </c>
@@ -4271,7 +3970,7 @@
       </c>
       <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="1:9" ht="32">
+    <row r="27" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>44925.328333333331</v>
       </c>
@@ -4298,32 +3997,32 @@
       </c>
       <c r="I27" s="17"/>
     </row>
-    <row r="28" spans="1:9" ht="33" thickBot="1">
-      <c r="A28" s="37" t="s">
+    <row r="28" spans="1:9" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="39"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="37"/>
       <c r="F28" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="G28" s="40"/>
-      <c r="H28" s="39"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="37"/>
       <c r="I28" s="16"/>
     </row>
-    <row r="29" spans="1:9" ht="15" customHeight="1">
-      <c r="A29" s="32" t="s">
+    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="34" t="s">
+      <c r="B29" s="31"/>
+      <c r="C29" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="D29" s="35"/>
-    </row>
-    <row r="30" spans="1:9" ht="48">
+      <c r="D29" s="33"/>
+    </row>
+    <row r="30" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
         <v>152</v>
       </c>
@@ -4337,7 +4036,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="33" thickBot="1">
+    <row r="31" spans="1:9" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
         <v>0</v>
       </c>
@@ -4374,14 +4073,14 @@
       <selection activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="6" width="11.5" style="23"/>
     <col min="7" max="7" width="27.5" style="23" customWidth="1"/>
     <col min="8" max="16384" width="11.5" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>154</v>
       </c>
@@ -4410,7 +4109,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>162</v>
       </c>
@@ -4436,7 +4135,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>162</v>
       </c>
@@ -4465,7 +4164,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>162</v>
       </c>
@@ -4497,7 +4196,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>162</v>
       </c>
@@ -4526,7 +4225,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>162</v>
       </c>
@@ -4555,7 +4254,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>162</v>
       </c>
@@ -4584,7 +4283,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>162</v>
       </c>
@@ -4613,7 +4312,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>162</v>
       </c>
@@ -4642,7 +4341,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>162</v>
       </c>
@@ -4671,7 +4370,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>162</v>
       </c>
@@ -4700,7 +4399,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>162</v>
       </c>
@@ -4729,7 +4428,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>162</v>
       </c>
@@ -4758,7 +4457,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>162</v>
       </c>
@@ -4787,7 +4486,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>162</v>
       </c>
@@ -4816,7 +4515,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>162</v>
       </c>
@@ -4845,7 +4544,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>162</v>
       </c>
@@ -4874,7 +4573,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>162</v>
       </c>
@@ -4903,7 +4602,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>162</v>
       </c>
@@ -4932,7 +4631,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>162</v>
       </c>
@@ -4961,7 +4660,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>162</v>
       </c>
@@ -4990,7 +4689,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>162</v>
       </c>
@@ -5019,7 +4718,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
         <v>162</v>
       </c>
@@ -5048,7 +4747,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
         <v>162</v>
       </c>
@@ -5077,7 +4776,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
         <v>162</v>
       </c>
@@ -5106,7 +4805,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
         <v>162</v>
       </c>
@@ -5135,7 +4834,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
         <v>162</v>
       </c>
@@ -5164,7 +4863,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
         <v>162</v>
       </c>
@@ -5193,7 +4892,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
         <v>162</v>
       </c>
@@ -5222,7 +4921,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
         <v>162</v>
       </c>
@@ -5251,7 +4950,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
         <v>162</v>
       </c>
@@ -5280,7 +4979,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
         <v>162</v>
       </c>
@@ -5309,7 +5008,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
         <v>162</v>
       </c>
@@ -5338,7 +5037,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
         <v>162</v>
       </c>
@@ -5367,7 +5066,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
         <v>162</v>
       </c>
@@ -5396,7 +5095,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
         <v>162</v>
       </c>
@@ -5425,7 +5124,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="23" t="s">
         <v>162</v>
       </c>
@@ -5454,7 +5153,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="23" t="s">
         <v>162</v>
       </c>
@@ -5483,7 +5182,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
         <v>162</v>
       </c>
@@ -5512,7 +5211,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
         <v>162</v>
       </c>
@@ -5541,7 +5240,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
         <v>162</v>
       </c>
@@ -5570,7 +5269,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="23" t="s">
         <v>162</v>
       </c>
@@ -5599,7 +5298,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="23" t="s">
         <v>162</v>
       </c>
@@ -5628,7 +5327,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
         <v>162</v>
       </c>
@@ -5657,7 +5356,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="23" t="s">
         <v>162</v>
       </c>
@@ -5686,7 +5385,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="23" t="s">
         <v>162</v>
       </c>
@@ -5715,7 +5414,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="23" t="s">
         <v>162</v>
       </c>
@@ -5744,7 +5443,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="23" t="s">
         <v>162</v>
       </c>
@@ -5773,7 +5472,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="23" t="s">
         <v>162</v>
       </c>
@@ -5802,7 +5501,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="23" t="s">
         <v>162</v>
       </c>
@@ -5831,7 +5530,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="23" t="s">
         <v>162</v>
       </c>
@@ -5860,7 +5559,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="23" t="s">
         <v>162</v>
       </c>
@@ -5889,7 +5588,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="23" t="s">
         <v>162</v>
       </c>
@@ -5918,7 +5617,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="23" t="s">
         <v>162</v>
       </c>
@@ -5947,7 +5646,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="23" t="s">
         <v>162</v>
       </c>
@@ -5976,7 +5675,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="23" t="s">
         <v>162</v>
       </c>
@@ -6005,7 +5704,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="23" t="s">
         <v>162</v>
       </c>
@@ -6034,7 +5733,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="23" t="s">
         <v>162</v>
       </c>
@@ -6063,7 +5762,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="23" t="s">
         <v>162</v>
       </c>
@@ -6092,7 +5791,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="23" t="s">
         <v>162</v>
       </c>
@@ -6121,7 +5820,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="23" t="s">
         <v>162</v>
       </c>
@@ -6150,7 +5849,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="23" t="s">
         <v>162</v>
       </c>
@@ -6179,7 +5878,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="23" t="s">
         <v>162</v>
       </c>
@@ -6208,7 +5907,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="s">
         <v>162</v>
       </c>
@@ -6237,7 +5936,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="23" t="s">
         <v>162</v>
       </c>
@@ -6266,7 +5965,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="23" t="s">
         <v>162</v>
       </c>
@@ -6295,7 +5994,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="23" t="s">
         <v>162</v>
       </c>
@@ -6324,7 +6023,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="23" t="s">
         <v>162</v>
       </c>
@@ -6353,7 +6052,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="23" t="s">
         <v>162</v>
       </c>
@@ -6382,7 +6081,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="23" t="s">
         <v>162</v>
       </c>
@@ -6411,7 +6110,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="23" t="s">
         <v>162</v>
       </c>
@@ -6440,7 +6139,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="23" t="s">
         <v>162</v>
       </c>
@@ -6469,7 +6168,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="23" t="s">
         <v>162</v>
       </c>
@@ -6498,7 +6197,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="23" t="s">
         <v>162</v>
       </c>
@@ -6527,7 +6226,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="23" t="s">
         <v>162</v>
       </c>
@@ -6556,7 +6255,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="23" t="s">
         <v>162</v>
       </c>
@@ -6585,7 +6284,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="23" t="s">
         <v>162</v>
       </c>
@@ -6614,7 +6313,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="23" t="s">
         <v>162</v>
       </c>
@@ -6643,7 +6342,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="23" t="s">
         <v>162</v>
       </c>
@@ -6672,7 +6371,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="23" t="s">
         <v>162</v>
       </c>
@@ -6701,7 +6400,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="23" t="s">
         <v>162</v>
       </c>
@@ -6730,7 +6429,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="23" t="s">
         <v>162</v>
       </c>

</xml_diff>